<commit_message>
Fixing some sheet usage
</commit_message>
<xml_diff>
--- a/calibration_5_colors_w_MEA_20230403.xlsx
+++ b/calibration_5_colors_w_MEA_20230403.xlsx
@@ -485,6 +485,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -505,6 +506,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -525,6 +527,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -545,6 +548,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -565,6 +569,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -585,6 +590,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -605,6 +611,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -625,6 +632,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -645,6 +653,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -665,6 +674,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -685,6 +695,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -705,6 +716,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -725,6 +737,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -745,6 +758,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -765,6 +779,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -785,6 +800,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -803,6 +819,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -932,11 +949,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="43522022"/>
-        <c:axId val="35000127"/>
+        <c:axId val="40592446"/>
+        <c:axId val="77391761"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43522022"/>
+        <c:axId val="40592446"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,11 +985,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35000127"/>
+        <c:crossAx val="77391761"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35000127"/>
+        <c:axId val="77391761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1031,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43522022"/>
+        <c:crossAx val="40592446"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1291,7 +1308,7 @@
             <c:idx val="16"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7e0021"/>
+                <a:srgbClr val="4a7ebb"/>
               </a:solidFill>
               <a:ln w="28440">
                 <a:solidFill>
@@ -1315,6 +1332,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1335,6 +1353,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1355,6 +1374,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1375,6 +1395,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1395,6 +1416,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1415,6 +1437,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1435,6 +1458,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1455,6 +1479,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1475,6 +1500,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1495,6 +1521,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1515,6 +1542,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1535,6 +1563,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1555,6 +1584,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1575,6 +1605,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1595,6 +1626,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1615,6 +1647,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1635,6 +1668,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1653,6 +1687,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1763,7 +1798,7 @@
                   <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.21</c:v>
+                  <c:v>0.196</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.219</c:v>
@@ -1785,11 +1820,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="4063739"/>
-        <c:axId val="54815804"/>
+        <c:axId val="24851609"/>
+        <c:axId val="59651040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4063739"/>
+        <c:axId val="24851609"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,11 +1856,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54815804"/>
+        <c:crossAx val="59651040"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54815804"/>
+        <c:axId val="59651040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1867,7 +1902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4063739"/>
+        <c:crossAx val="24851609"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2154,6 +2189,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2174,6 +2210,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2194,6 +2231,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2214,6 +2252,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2234,6 +2273,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2254,6 +2294,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2274,6 +2315,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2294,6 +2336,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2314,6 +2357,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2334,6 +2378,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2354,6 +2399,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2374,6 +2420,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2394,6 +2441,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2414,6 +2462,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2434,6 +2483,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2454,6 +2504,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -2472,6 +2523,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2601,11 +2653,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="17490089"/>
-        <c:axId val="35226831"/>
+        <c:axId val="23236805"/>
+        <c:axId val="91615137"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17490089"/>
+        <c:axId val="23236805"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2637,11 +2689,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35226831"/>
+        <c:crossAx val="91615137"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35226831"/>
+        <c:axId val="91615137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2683,7 +2735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17490089"/>
+        <c:crossAx val="23236805"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2748,10 +2800,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127538638395708"/>
-          <c:y val="0.051434103836379"/>
-          <c:w val="0.675437476050581"/>
-          <c:h val="0.797410141595062"/>
+          <c:x val="0.127521062037273"/>
+          <c:y val="0.051440329218107"/>
+          <c:w val="0.675389328567781"/>
+          <c:h val="0.797264584846284"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2981,6 +3033,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3001,6 +3054,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3021,6 +3075,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3041,6 +3096,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3061,6 +3117,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3081,6 +3138,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3101,6 +3159,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3121,6 +3180,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3141,6 +3201,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3161,6 +3222,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3181,6 +3243,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3201,6 +3264,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3221,6 +3285,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3241,6 +3306,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3261,6 +3327,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3281,6 +3348,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3299,6 +3367,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3428,11 +3497,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91433228"/>
-        <c:axId val="58766384"/>
+        <c:axId val="41257559"/>
+        <c:axId val="13080789"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91433228"/>
+        <c:axId val="41257559"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3464,11 +3533,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58766384"/>
+        <c:crossAx val="13080789"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58766384"/>
+        <c:axId val="13080789"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +3579,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91433228"/>
+        <c:crossAx val="41257559"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3797,6 +3866,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3817,6 +3887,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3837,6 +3908,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3857,6 +3929,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3877,6 +3950,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3897,6 +3971,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3917,6 +3992,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3937,6 +4013,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3957,6 +4034,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3977,6 +4055,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3997,6 +4076,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4017,6 +4097,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4037,6 +4118,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4057,6 +4139,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4077,6 +4160,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4097,6 +4181,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4115,6 +4200,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4244,11 +4330,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="81674879"/>
-        <c:axId val="27492598"/>
+        <c:axId val="18469973"/>
+        <c:axId val="31887442"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81674879"/>
+        <c:axId val="18469973"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4280,11 +4366,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27492598"/>
+        <c:crossAx val="31887442"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27492598"/>
+        <c:axId val="31887442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4326,7 +4412,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81674879"/>
+        <c:crossAx val="18469973"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4613,6 +4699,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4633,6 +4720,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4653,6 +4741,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4673,6 +4762,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4693,6 +4783,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4713,6 +4804,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4733,6 +4825,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4753,6 +4846,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4773,6 +4867,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4793,6 +4888,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4813,6 +4909,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4833,6 +4930,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4853,6 +4951,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4873,6 +4972,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4893,6 +4993,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4913,6 +5014,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4931,6 +5033,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -5060,11 +5163,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="42797945"/>
-        <c:axId val="66063417"/>
+        <c:axId val="45707909"/>
+        <c:axId val="4692987"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42797945"/>
+        <c:axId val="45707909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5096,11 +5199,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66063417"/>
+        <c:crossAx val="4692987"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66063417"/>
+        <c:axId val="4692987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5142,7 +5245,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42797945"/>
+        <c:crossAx val="45707909"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -5429,6 +5532,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5449,6 +5553,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5469,6 +5574,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5489,6 +5595,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5509,6 +5616,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5529,6 +5637,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5549,6 +5658,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5569,6 +5679,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5589,6 +5700,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5609,6 +5721,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5629,6 +5742,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5649,6 +5763,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5669,6 +5784,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5689,6 +5805,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5709,6 +5826,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5729,6 +5847,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -5747,6 +5866,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -5876,11 +5996,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="49914063"/>
-        <c:axId val="44757806"/>
+        <c:axId val="20211698"/>
+        <c:axId val="79810110"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49914063"/>
+        <c:axId val="20211698"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5912,11 +6032,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44757806"/>
+        <c:crossAx val="79810110"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44757806"/>
+        <c:axId val="79810110"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5958,7 +6078,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49914063"/>
+        <c:crossAx val="20211698"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6023,10 +6143,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127538638395708"/>
-          <c:y val="0.051434103836379"/>
-          <c:w val="0.675437476050581"/>
-          <c:h val="0.797410141595062"/>
+          <c:x val="0.127521062037273"/>
+          <c:y val="0.051440329218107"/>
+          <c:w val="0.675389328567781"/>
+          <c:h val="0.797264584846284"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6256,6 +6376,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6276,6 +6397,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6296,6 +6418,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6316,6 +6439,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6336,6 +6460,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6356,6 +6481,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6376,6 +6502,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6396,6 +6523,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6416,6 +6544,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6436,6 +6565,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6456,6 +6586,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6476,6 +6607,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6496,6 +6628,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6516,6 +6649,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6536,6 +6670,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6556,6 +6691,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -6574,6 +6710,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -6703,11 +6840,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="133834"/>
-        <c:axId val="42922469"/>
+        <c:axId val="85262289"/>
+        <c:axId val="88494872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133834"/>
+        <c:axId val="85262289"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6739,11 +6876,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42922469"/>
+        <c:crossAx val="88494872"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42922469"/>
+        <c:axId val="88494872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6785,7 +6922,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133834"/>
+        <c:crossAx val="85262289"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -7072,6 +7209,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7092,6 +7230,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7112,6 +7251,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7132,6 +7272,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7152,6 +7293,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7172,6 +7314,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7192,6 +7335,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7212,6 +7356,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7232,6 +7377,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7252,6 +7398,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7272,6 +7419,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7292,6 +7440,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7312,6 +7461,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7332,6 +7482,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7352,6 +7503,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7372,6 +7524,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7390,6 +7543,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -7519,11 +7673,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="72353768"/>
-        <c:axId val="16567670"/>
+        <c:axId val="81267260"/>
+        <c:axId val="50570325"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72353768"/>
+        <c:axId val="81267260"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7555,11 +7709,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16567670"/>
+        <c:crossAx val="50570325"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16567670"/>
+        <c:axId val="50570325"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7601,7 +7755,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72353768"/>
+        <c:crossAx val="81267260"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -7888,6 +8042,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7908,6 +8063,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7928,6 +8084,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7948,6 +8105,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7968,6 +8126,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -7988,6 +8147,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8008,6 +8168,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8028,6 +8189,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8048,6 +8210,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8068,6 +8231,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8088,6 +8252,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8108,6 +8273,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8128,6 +8294,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8148,6 +8315,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8168,6 +8336,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8188,6 +8357,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="r"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -8206,6 +8376,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -8335,11 +8506,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="84126504"/>
-        <c:axId val="28389253"/>
+        <c:axId val="87390623"/>
+        <c:axId val="67981906"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84126504"/>
+        <c:axId val="87390623"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8371,11 +8542,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28389253"/>
+        <c:crossAx val="67981906"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="28389253"/>
+        <c:axId val="67981906"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8417,7 +8588,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84126504"/>
+        <c:crossAx val="87390623"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -8481,9 +8652,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>264600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8491,8 +8662,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10060560" y="1828800"/>
-        <a:ext cx="5635440" cy="2974680"/>
+        <a:off x="10064880" y="1828800"/>
+        <a:ext cx="5639040" cy="2974320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8511,9 +8682,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>284040</xdr:colOff>
+      <xdr:colOff>283680</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8521,8 +8692,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10079640" y="5562000"/>
-        <a:ext cx="5635440" cy="2973600"/>
+        <a:off x="10083960" y="5562000"/>
+        <a:ext cx="5639040" cy="2973240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8541,9 +8712,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>360360</xdr:colOff>
+      <xdr:colOff>360000</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8551,8 +8722,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10154880" y="9247320"/>
-        <a:ext cx="5636520" cy="2974320"/>
+        <a:off x="10159200" y="9247320"/>
+        <a:ext cx="5640120" cy="2973960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8571,9 +8742,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>190800</xdr:colOff>
+      <xdr:colOff>190440</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8582,7 +8753,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="927000" y="9999360"/>
-        <a:ext cx="5880960" cy="3622320"/>
+        <a:ext cx="5883840" cy="3621960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8601,9 +8772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>278280</xdr:colOff>
+      <xdr:colOff>277920</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8612,7 +8783,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="309600" y="5380560"/>
-        <a:ext cx="5646240" cy="3324960"/>
+        <a:ext cx="5648400" cy="3324600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8636,9 +8807,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
+      <xdr:colOff>264600</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>40680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8646,8 +8817,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10695600" y="1828800"/>
-        <a:ext cx="5635440" cy="2974680"/>
+        <a:off x="10700640" y="1828800"/>
+        <a:ext cx="5639040" cy="2974320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8666,9 +8837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>360360</xdr:colOff>
+      <xdr:colOff>360000</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8676,8 +8847,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10789920" y="9247320"/>
-        <a:ext cx="5636520" cy="2974320"/>
+        <a:off x="10794960" y="9247320"/>
+        <a:ext cx="5640120" cy="2973960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8696,9 +8867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>422280</xdr:colOff>
+      <xdr:colOff>421920</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8707,7 +8878,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="927000" y="9999360"/>
-        <a:ext cx="5807880" cy="3622320"/>
+        <a:ext cx="5810760" cy="3621960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8726,9 +8897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>509760</xdr:colOff>
+      <xdr:colOff>509400</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8737,7 +8908,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="309600" y="5380560"/>
-        <a:ext cx="5572800" cy="3324960"/>
+        <a:ext cx="5574960" cy="3324600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8756,9 +8927,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>662400</xdr:colOff>
+      <xdr:colOff>662040</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>100080</xdr:rowOff>
+      <xdr:rowOff>99720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8766,8 +8937,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8177400" y="5347800"/>
-        <a:ext cx="5731560" cy="3324960"/>
+        <a:off x="8181360" y="5347800"/>
+        <a:ext cx="5734440" cy="3324600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8788,10 +8959,10 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O29" activeCellId="1" sqref="C4:C20 O29"/>
+      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
@@ -9328,10 +9499,10 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4:C20"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
@@ -9647,7 +9818,7 @@
         <v>13.47</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>0.21</v>
+        <v>0.196</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>0.135</v>

</xml_diff>

<commit_message>
Testing with new leds
</commit_message>
<xml_diff>
--- a/calibration_5_colors_w_MEA_20230403.xlsx
+++ b/calibration_5_colors_w_MEA_20230403.xlsx
@@ -86,7 +86,7 @@
     <t xml:space="preserve">Violet</t>
   </si>
   <si>
-    <t xml:space="preserve">test</t>
+    <t xml:space="preserve">595xDM605xF600</t>
   </si>
   <si>
     <t xml:space="preserve">MEA3_625</t>
@@ -269,7 +269,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart209.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -967,11 +967,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="91016903"/>
-        <c:axId val="9023323"/>
+        <c:axId val="86329484"/>
+        <c:axId val="28123379"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91016903"/>
+        <c:axId val="86329484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,11 +1003,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9023323"/>
+        <c:crossAx val="28123379"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9023323"/>
+        <c:axId val="28123379"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1049,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91016903"/>
+        <c:crossAx val="86329484"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1102,7 +1102,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart210.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1800,11 +1800,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="54247912"/>
-        <c:axId val="37240154"/>
+        <c:axId val="96677909"/>
+        <c:axId val="3776001"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54247912"/>
+        <c:axId val="96677909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,11 +1836,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37240154"/>
+        <c:crossAx val="3776001"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37240154"/>
+        <c:axId val="3776001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,7 +1882,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54247912"/>
+        <c:crossAx val="96677909"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1935,7 +1935,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart211.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1947,10 +1947,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127511641257894"/>
-          <c:y val="0.0514465561070088"/>
-          <c:w val="0.675320533265293"/>
-          <c:h val="0.797118992858007"/>
+          <c:x val="0.127476587883035"/>
+          <c:y val="0.051459014408524"/>
+          <c:w val="0.675224565203542"/>
+          <c:h val="0.796827703111757"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2644,11 +2644,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83792116"/>
-        <c:axId val="98943065"/>
+        <c:axId val="21878783"/>
+        <c:axId val="43302312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83792116"/>
+        <c:axId val="21878783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2680,11 +2680,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98943065"/>
+        <c:crossAx val="43302312"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98943065"/>
+        <c:axId val="43302312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2726,7 +2726,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83792116"/>
+        <c:crossAx val="21878783"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2779,7 +2779,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart212.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3477,11 +3477,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="60445241"/>
-        <c:axId val="9146063"/>
+        <c:axId val="99295255"/>
+        <c:axId val="41207393"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60445241"/>
+        <c:axId val="99295255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3513,11 +3513,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9146063"/>
+        <c:crossAx val="41207393"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9146063"/>
+        <c:axId val="41207393"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3559,7 +3559,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60445241"/>
+        <c:crossAx val="99295255"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3612,7 +3612,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart213.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4310,11 +4310,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="2893539"/>
-        <c:axId val="69015537"/>
+        <c:axId val="88529595"/>
+        <c:axId val="85537513"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2893539"/>
+        <c:axId val="88529595"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4346,11 +4346,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69015537"/>
+        <c:crossAx val="85537513"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69015537"/>
+        <c:axId val="85537513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4392,7 +4392,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2893539"/>
+        <c:crossAx val="88529595"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4445,7 +4445,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart214.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5143,11 +5143,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="93135459"/>
-        <c:axId val="86477818"/>
+        <c:axId val="6919624"/>
+        <c:axId val="25049151"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93135459"/>
+        <c:axId val="6919624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5179,11 +5179,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86477818"/>
+        <c:crossAx val="25049151"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86477818"/>
+        <c:axId val="25049151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5225,7 +5225,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93135459"/>
+        <c:crossAx val="6919624"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -5278,7 +5278,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart215.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5290,10 +5290,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.127503508100523"/>
-          <c:y val="0.0514465561070088"/>
-          <c:w val="0.675341242505422"/>
-          <c:h val="0.797118992858007"/>
+          <c:x val="0.127476587883035"/>
+          <c:y val="0.051459014408524"/>
+          <c:w val="0.675224565203542"/>
+          <c:h val="0.796827703111757"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5987,11 +5987,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71749866"/>
-        <c:axId val="20233819"/>
+        <c:axId val="97967751"/>
+        <c:axId val="16872181"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71749866"/>
+        <c:axId val="97967751"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6023,11 +6023,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20233819"/>
+        <c:crossAx val="16872181"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20233819"/>
+        <c:axId val="16872181"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6069,7 +6069,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71749866"/>
+        <c:crossAx val="97967751"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6122,7 +6122,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart216.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6820,11 +6820,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="54818235"/>
-        <c:axId val="19689148"/>
+        <c:axId val="25006036"/>
+        <c:axId val="86193447"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54818235"/>
+        <c:axId val="25006036"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6856,11 +6856,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19689148"/>
+        <c:crossAx val="86193447"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="19689148"/>
+        <c:axId val="86193447"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6902,7 +6902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54818235"/>
+        <c:crossAx val="25006036"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6955,7 +6955,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart217.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7653,11 +7653,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="50586479"/>
-        <c:axId val="81372338"/>
+        <c:axId val="87317137"/>
+        <c:axId val="44139172"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50586479"/>
+        <c:axId val="87317137"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7689,11 +7689,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81372338"/>
+        <c:crossAx val="44139172"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81372338"/>
+        <c:axId val="44139172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7735,7 +7735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50586479"/>
+        <c:crossAx val="87317137"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -7799,9 +7799,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>40320</xdr:rowOff>
+      <xdr:rowOff>39600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7809,8 +7809,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10069560" y="1828800"/>
-        <a:ext cx="5642280" cy="2973960"/>
+        <a:off x="10078200" y="1828800"/>
+        <a:ext cx="5649480" cy="2973240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7829,9 +7829,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>282600</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>152280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7839,8 +7839,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10088640" y="5562000"/>
-        <a:ext cx="5642280" cy="2972880"/>
+        <a:off x="10097280" y="5562000"/>
+        <a:ext cx="5649480" cy="2972160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7859,9 +7859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>359640</xdr:colOff>
+      <xdr:colOff>358920</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7869,8 +7869,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10163880" y="9247320"/>
-        <a:ext cx="5643360" cy="2973600"/>
+        <a:off x="10172520" y="9247320"/>
+        <a:ext cx="5650560" cy="2972880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7889,9 +7889,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>190080</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7900,7 +7900,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="927000" y="9999360"/>
-        <a:ext cx="5886720" cy="3621600"/>
+        <a:ext cx="5892480" cy="3620880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7919,9 +7919,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>276840</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7930,7 +7930,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="309600" y="5380560"/>
-        <a:ext cx="5650560" cy="3324240"/>
+        <a:ext cx="5654880" cy="3323520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7954,9 +7954,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7964,8 +7964,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10350720" y="1691640"/>
-        <a:ext cx="5642640" cy="2973960"/>
+        <a:off x="10360800" y="1691640"/>
+        <a:ext cx="5649480" cy="2973240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7984,9 +7984,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>359640</xdr:colOff>
+      <xdr:colOff>358920</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>97560</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7994,8 +7994,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10445040" y="8515800"/>
-        <a:ext cx="5643720" cy="2973600"/>
+        <a:off x="10455120" y="8515800"/>
+        <a:ext cx="5650560" cy="2972880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8014,9 +8014,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>421560</xdr:colOff>
+      <xdr:colOff>420840</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>33480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8025,7 +8025,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="927000" y="9206640"/>
-        <a:ext cx="5812920" cy="3621600"/>
+        <a:ext cx="5817240" cy="3620880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8044,9 +8044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>509040</xdr:colOff>
+      <xdr:colOff>508320</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>39960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8055,7 +8055,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="309600" y="4953600"/>
-        <a:ext cx="5576760" cy="3324240"/>
+        <a:ext cx="5579640" cy="3323520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8063,21 +8063,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>925200</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>75240</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>7920</xdr:rowOff>
-    </xdr:to>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8094,7 +8079,7 @@
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.57"/>
@@ -8634,7 +8619,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.72"/>
   </cols>
@@ -8679,7 +8664,7 @@
       <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="J2" s="2"/>
@@ -8745,7 +8730,7 @@
         <v>0.0023</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>0.0023</v>
+        <v>0</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="2"/>
@@ -8774,7 +8759,7 @@
         <v>0.0113</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>0.0113</v>
+        <v>0.069</v>
       </c>
       <c r="H6" s="1"/>
       <c r="J6" s="2"/>
@@ -8803,7 +8788,7 @@
         <v>0.0215</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>0.0215</v>
+        <v>0.172</v>
       </c>
       <c r="H7" s="1"/>
       <c r="J7" s="2"/>
@@ -8832,7 +8817,7 @@
         <v>0.0358</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.0358</v>
+        <v>0.33</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -8856,7 +8841,7 @@
         <v>0.135</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>0.135</v>
+        <v>1.42</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -8880,7 +8865,7 @@
         <v>0.238</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>0.238</v>
+        <v>2.56</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -8904,7 +8889,7 @@
         <v>0.341</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>0.341</v>
+        <v>3.72</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -8928,7 +8913,7 @@
         <v>0.494</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>0.494</v>
+        <v>5.42</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -8952,7 +8937,7 @@
         <v>0.747</v>
       </c>
       <c r="G13" s="1" t="n">
-        <v>0.747</v>
+        <v>8.21</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -8976,7 +8961,7 @@
         <v>0.994</v>
       </c>
       <c r="G14" s="1" t="n">
-        <v>0.994</v>
+        <v>10.9</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -9000,7 +8985,7 @@
         <v>1.239</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>1.239</v>
+        <v>13.47</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -9024,7 +9009,7 @@
         <v>1.477</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>1.477</v>
+        <v>15.9</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -9048,7 +9033,7 @@
         <v>1.714</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>2</v>
+        <v>18.14</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -9072,7 +9057,7 @@
         <v>1.943</v>
       </c>
       <c r="G18" s="1" t="n">
-        <v>3</v>
+        <v>20.22</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -9096,7 +9081,7 @@
         <v>2.175</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>4</v>
+        <v>21.98</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -9120,7 +9105,7 @@
         <v>2.343</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>5</v>
+        <v>23.43</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -9147,7 +9132,7 @@
         <v>26</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9169,8 +9154,8 @@
       <c r="F23" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>100</v>
+      <c r="G23" s="0" t="n">
+        <v>7500</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9199,7 +9184,7 @@
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">G23/G20</f>
-        <v>20</v>
+        <v>320.102432778489</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9208,7 +9193,6 @@
       </c>
       <c r="C25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">

</xml_diff>